<commit_message>
feat. QuizDataController & SoundDataController
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -105,6 +105,22 @@
   </si>
   <si>
     <t xml:space="preserve">//sound도 index랑 동일하게 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>option_02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>option_03</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wrongOption</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -446,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -461,7 +477,7 @@
     <col min="7" max="7" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -477,8 +493,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -492,13 +511,16 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -514,11 +536,14 @@
       <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>6</v>
       </c>
@@ -534,8 +559,11 @@
       <c r="F4" t="s">
         <v>16</v>
       </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -550,6 +578,9 @@
       </c>
       <c r="F5" t="s">
         <v>19</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat. soundRecognize & quizData
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
@@ -24,16 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -42,10 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>option_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>어떤 소리인지 맞춰보세요1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -58,22 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>option_02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>option_03</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>n</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>wrongOption</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>owl</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,13 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>정답x_01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정답x_02</t>
-  </si>
-  <si>
     <t>폭포</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,7 +148,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>QuizSound/</t>
+    <t>QuizSound/test01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuizSound/test02</t>
+  </si>
+  <si>
+    <t>quizName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>correctAnswer</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -532,270 +512,197 @@
     <col min="2" max="2" width="23.25" customWidth="1"/>
     <col min="3" max="3" width="27.375" customWidth="1"/>
     <col min="4" max="4" width="17.25" customWidth="1"/>
-    <col min="5" max="5" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="27.75" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="29.375" customWidth="1"/>
     <col min="8" max="8" width="27.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="1" t="s">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6">
-        <v>2</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8">
-        <v>2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="17.25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
feat. sound/ effect ect
</commit_message>
<xml_diff>
--- a/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
+++ b/WhiteCane/Assets/Resources/Xlsx/QuizData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>array</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -42,10 +42,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>어떤 소리인지 맞춰보세요2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>어떤 소리인지 맞춰보세요3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -76,10 +72,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>폭포</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>그네</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -100,10 +92,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>버섯</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부엉이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -112,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>falls</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>pond</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,10 +120,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>mushroom</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>s</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -160,6 +140,17 @@
   </si>
   <si>
     <t>correctAnswer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bush</t>
+  </si>
+  <si>
+    <t>bush</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>덤불</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -501,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -528,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -536,173 +527,156 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>27</v>
       </c>
-      <c r="E6" t="s">
-        <v>33</v>
-      </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
         <v>28</v>
       </c>
-      <c r="E9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="F9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="D12" s="1"/>
+        <v>27</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="D11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>